<commit_message>
added CuttingData compacted version
</commit_message>
<xml_diff>
--- a/templates/cuttingData.xlsx
+++ b/templates/cuttingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdel\OneDrive\Desktop\yazaki\xlsx git\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352F8C57-079A-4580-8C9A-5A3FD648AA34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA33369-F558-4C0F-AAFB-D6641904CABF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wire list" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="63">
   <si>
     <t>Customer Module/Option</t>
   </si>
@@ -197,6 +197,24 @@
   </si>
   <si>
     <t>SK</t>
+  </si>
+  <si>
+    <t>DOUBLE PM</t>
+  </si>
+  <si>
+    <t>DOUBLE SK</t>
+  </si>
+  <si>
+    <t>TWIST SK</t>
+  </si>
+  <si>
+    <t>TWIST PM</t>
+  </si>
+  <si>
+    <t>SPLICE PM</t>
+  </si>
+  <si>
+    <t>SPLICE SK</t>
   </si>
 </sst>
 </file>
@@ -826,10 +844,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{919D6D6A-E967-4CE1-8374-9A79EF170A67}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:BH1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,115 +859,240 @@
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BE1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>52</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -959,223 +1102,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F9024B-8312-444B-B007-E5FDA8C2AC15}">
-  <dimension ref="A1:BF1"/>
-  <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E55EEA-2974-4E0C-9F9C-E206962A3CDA}">
-  <dimension ref="A1:BF1"/>
+  <dimension ref="A1:BH1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1187,56 +1117,59 @@
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1265,150 +1198,415 @@
         <v>56</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E55EEA-2974-4E0C-9F9C-E206962A3CDA}">
+  <dimension ref="A1:BH1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="K1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>